<commit_message>
fixed WIT and combination and re ran WIT 2000 and 6000
</commit_message>
<xml_diff>
--- a/baseline-2000-simulation.xlsx
+++ b/baseline-2000-simulation.xlsx
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>10314.97486662847</v>
+        <v>10314.9748666943</v>
       </c>
       <c r="C2" t="n">
-        <v>1137.048602730748</v>
+        <v>1137.048602726682</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>51.57123316032897</v>
+        <v>51.5712332008092</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +477,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>9947.64671247675</v>
+        <v>9947.646712402227</v>
       </c>
       <c r="C3" t="n">
-        <v>1061.346475639645</v>
+        <v>1061.346475676937</v>
       </c>
       <c r="D3" t="n">
-        <v>0.006805081099477522</v>
+        <v>0.006805118321489547</v>
       </c>
       <c r="E3" t="n">
-        <v>26.78177048457937</v>
+        <v>26.78177026421556</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +494,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>9734.025418823663</v>
+        <v>9734.02541891311</v>
       </c>
       <c r="C4" t="n">
-        <v>1091.968199528717</v>
+        <v>1091.968199483623</v>
       </c>
       <c r="D4" t="n">
-        <v>0.006375275333861997</v>
+        <v>0.006375231074269022</v>
       </c>
       <c r="E4" t="n">
-        <v>26.02800966207883</v>
+        <v>26.02800959731272</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +511,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>9971.483682245875</v>
+        <v>9971.483682252787</v>
       </c>
       <c r="C5" t="n">
-        <v>846.6020591828438</v>
+        <v>846.602059182077</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>26.50099764327704</v>
+        <v>26.50099775499366</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +528,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>9725.027084493246</v>
+        <v>9725.027084846626</v>
       </c>
       <c r="C6" t="n">
-        <v>1393.17968066077</v>
+        <v>1393.17968063906</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>25.76524434616047</v>
+        <v>25.76524447824248</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>11155.88934668586</v>
+        <v>11155.88934667704</v>
       </c>
       <c r="C7" t="n">
-        <v>1086.110163171495</v>
+        <v>1086.110163175937</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0004896523381989865</v>
+        <v>0.0004896566943561153</v>
       </c>
       <c r="E7" t="n">
-        <v>34.14174946892019</v>
+        <v>34.14174944561099</v>
       </c>
     </row>
     <row r="8">
@@ -562,16 +562,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>13157.2034921647</v>
+        <v>13157.2034921371</v>
       </c>
       <c r="C8" t="n">
-        <v>1131.045467196581</v>
+        <v>1131.045467197823</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>1239.947156061476</v>
+        <v>1239.947156779721</v>
       </c>
     </row>
     <row r="9">
@@ -579,16 +579,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>14369.81370475614</v>
+        <v>14369.81370476277</v>
       </c>
       <c r="C9" t="n">
-        <v>1423.190263591437</v>
+        <v>1423.190263590973</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>59.94034989478433</v>
+        <v>59.94034989416571</v>
       </c>
     </row>
     <row r="10">
@@ -596,16 +596,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>15340.79804167667</v>
+        <v>15340.79804168605</v>
       </c>
       <c r="C10" t="n">
-        <v>956.2272091789559</v>
+        <v>956.2272091782542</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>90.91160535563013</v>
+        <v>90.91160536326501</v>
       </c>
     </row>
     <row r="11">
@@ -613,16 +613,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>15797.18773679917</v>
+        <v>15797.18773679134</v>
       </c>
       <c r="C11" t="n">
-        <v>688.4650688544169</v>
+        <v>688.4650688550507</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>116.4330240771519</v>
+        <v>116.4330266416747</v>
       </c>
     </row>
     <row r="12">
@@ -630,16 +630,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>15601.15297746795</v>
+        <v>15601.15297747264</v>
       </c>
       <c r="C12" t="n">
-        <v>1004.850375964953</v>
+        <v>1004.850375962612</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>910.9333640403597</v>
+        <v>910.9333641683695</v>
       </c>
     </row>
     <row r="13">
@@ -647,16 +647,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>15712.61000188935</v>
+        <v>15712.61000189716</v>
       </c>
       <c r="C13" t="n">
-        <v>907.3925053661386</v>
+        <v>907.3925053655673</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>92.39038070696125</v>
+        <v>92.39038072610721</v>
       </c>
     </row>
     <row r="14">
@@ -664,16 +664,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>15500.16411850929</v>
+        <v>15500.16411848887</v>
       </c>
       <c r="C14" t="n">
-        <v>1013.877472890957</v>
+        <v>1013.87747289314</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>91.25624113660288</v>
+        <v>91.25624111995516</v>
       </c>
     </row>
     <row r="15">
@@ -681,16 +681,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>15354.30873048629</v>
+        <v>15354.30873047258</v>
       </c>
       <c r="C15" t="n">
-        <v>1131.688004282093</v>
+        <v>1131.688004289036</v>
       </c>
       <c r="D15" t="n">
-        <v>0.003261970009921589</v>
+        <v>0.003261976764009644</v>
       </c>
       <c r="E15" t="n">
-        <v>90.86189643559672</v>
+        <v>90.86189641642432</v>
       </c>
     </row>
     <row r="16">
@@ -698,16 +698,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>15371.35912044981</v>
+        <v>15371.35912044596</v>
       </c>
       <c r="C16" t="n">
-        <v>1053.647544935588</v>
+        <v>1053.647544935976</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>90.91234334064438</v>
+        <v>90.91234335432918</v>
       </c>
     </row>
     <row r="17">
@@ -715,16 +715,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>15128.14611300894</v>
+        <v>15128.14611300899</v>
       </c>
       <c r="C17" t="n">
-        <v>1349.853874555657</v>
+        <v>1349.853874555499</v>
       </c>
       <c r="D17" t="n">
-        <v>1.242294454287938e-05</v>
+        <v>1.242309651062072e-05</v>
       </c>
       <c r="E17" t="n">
-        <v>62.35332109115862</v>
+        <v>62.35332109201857</v>
       </c>
     </row>
     <row r="18">
@@ -732,16 +732,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>15270.67629117678</v>
+        <v>15270.67629117658</v>
       </c>
       <c r="C18" t="n">
-        <v>1564.323703383565</v>
+        <v>1564.323703383784</v>
       </c>
       <c r="D18" t="n">
-        <v>5.434230135940606e-06</v>
+        <v>5.434144284675447e-06</v>
       </c>
       <c r="E18" t="n">
-        <v>90.44374637371253</v>
+        <v>90.44374637281221</v>
       </c>
     </row>
     <row r="19">
@@ -749,16 +749,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>15766.68316405887</v>
+        <v>15766.6831640604</v>
       </c>
       <c r="C19" t="n">
-        <v>1519.572910483553</v>
+        <v>1519.572910483477</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>608.2576024935098</v>
+        <v>608.2576035579182</v>
       </c>
     </row>
     <row r="20">
@@ -766,16 +766,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>16005.92879864901</v>
+        <v>16005.92879864927</v>
       </c>
       <c r="C20" t="n">
-        <v>1759.070984809125</v>
+        <v>1759.070984808802</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0002163255728236439</v>
+        <v>0.0002163255640336022</v>
       </c>
       <c r="E20" t="n">
-        <v>95.65616642065611</v>
+        <v>95.65616642330393</v>
       </c>
     </row>
     <row r="21">
@@ -783,16 +783,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>15889.56852839544</v>
+        <v>15889.5685283967</v>
       </c>
       <c r="C21" t="n">
-        <v>1694.429207426035</v>
+        <v>1694.429207425525</v>
       </c>
       <c r="D21" t="n">
-        <v>0.002261916883871207</v>
+        <v>0.002261916095761431</v>
       </c>
       <c r="E21" t="n">
-        <v>93.04986107150128</v>
+        <v>93.04986104571222</v>
       </c>
     </row>
     <row r="22">
@@ -800,16 +800,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>16387.60041949287</v>
+        <v>16387.60041945793</v>
       </c>
       <c r="C22" t="n">
-        <v>446.3618984541394</v>
+        <v>446.3618984716046</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0376444119207479</v>
+        <v>0.03764442928824073</v>
       </c>
       <c r="E22" t="n">
-        <v>302.9142599525489</v>
+        <v>302.9142600071825</v>
       </c>
     </row>
     <row r="23">
@@ -817,16 +817,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>14963.04076582207</v>
+        <v>14963.04076582164</v>
       </c>
       <c r="C23" t="n">
-        <v>653.9587157255914</v>
+        <v>653.9587157258545</v>
       </c>
       <c r="D23" t="n">
-        <v>0.000517934449109671</v>
+        <v>0.000517934630700982</v>
       </c>
       <c r="E23" t="n">
-        <v>61.34437743732167</v>
+        <v>61.34437743755075</v>
       </c>
     </row>
     <row r="24">
@@ -834,16 +834,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>13154.66254754587</v>
+        <v>13154.66254754612</v>
       </c>
       <c r="C24" t="n">
-        <v>861.3373572994594</v>
+        <v>861.3373572994135</v>
       </c>
       <c r="D24" t="n">
-        <v>9.50596308671838e-05</v>
+        <v>9.505941462090065e-05</v>
       </c>
       <c r="E24" t="n">
-        <v>59.91194385721796</v>
+        <v>59.9119438564006</v>
       </c>
     </row>
     <row r="25">
@@ -851,16 +851,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>11515.70061789801</v>
+        <v>11515.70061789718</v>
       </c>
       <c r="C25" t="n">
-        <v>1086.299490627063</v>
+        <v>1086.299490627188</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>51.15548677062948</v>
+        <v>51.1554867700262</v>
       </c>
     </row>
     <row r="26">
@@ -868,16 +868,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>10516.22386765285</v>
+        <v>10516.22386768298</v>
       </c>
       <c r="C26" t="n">
-        <v>1167.776356149133</v>
+        <v>1167.776356146613</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>28.55176974143971</v>
+        <v>28.55176973905816</v>
       </c>
     </row>
     <row r="27">
@@ -885,16 +885,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>10291.22831047777</v>
+        <v>10291.22831047386</v>
       </c>
       <c r="C27" t="n">
-        <v>922.7701046357104</v>
+        <v>922.7701046375972</v>
       </c>
       <c r="D27" t="n">
-        <v>0.001583304120872469</v>
+        <v>0.001583306087601723</v>
       </c>
       <c r="E27" t="n">
-        <v>27.47038788581195</v>
+        <v>27.4703878884276</v>
       </c>
     </row>
     <row r="28">
@@ -902,16 +902,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>9890.534589718871</v>
+        <v>9890.534589736231</v>
       </c>
       <c r="C28" t="n">
-        <v>1109.464623259698</v>
+        <v>1109.464623251005</v>
       </c>
       <c r="D28" t="n">
-        <v>0.0007862370897266928</v>
+        <v>0.0007862284141238685</v>
       </c>
       <c r="E28" t="n">
-        <v>26.33903455348626</v>
+        <v>26.33903455098085</v>
       </c>
     </row>
     <row r="29">
@@ -919,16 +919,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>9968.426845217222</v>
+        <v>9968.42684502972</v>
       </c>
       <c r="C29" t="n">
-        <v>972.5803492185033</v>
+        <v>972.5803492296609</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>26.50434053459016</v>
+        <v>26.50434053501909</v>
       </c>
     </row>
     <row r="30">
@@ -936,16 +936,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>10400.39683631672</v>
+        <v>10400.39683631506</v>
       </c>
       <c r="C30" t="n">
-        <v>838.5985099845331</v>
+        <v>838.5985099858423</v>
       </c>
       <c r="D30" t="n">
-        <v>0.004649052420329657</v>
+        <v>0.004649052765824817</v>
       </c>
       <c r="E30" t="n">
-        <v>28.03060907495322</v>
+        <v>28.03060906949516</v>
       </c>
     </row>
     <row r="31">
@@ -953,16 +953,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>11187.44340950149</v>
+        <v>11187.44340950525</v>
       </c>
       <c r="C31" t="n">
-        <v>1149.559321394757</v>
+        <v>1149.559321394358</v>
       </c>
       <c r="D31" t="n">
-        <v>6.52768648318388e-05</v>
+        <v>6.527578892230699e-05</v>
       </c>
       <c r="E31" t="n">
-        <v>35.13307144877329</v>
+        <v>35.13307144832248</v>
       </c>
     </row>
     <row r="32">
@@ -970,16 +970,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>13316.34623032133</v>
+        <v>13316.34623033222</v>
       </c>
       <c r="C32" t="n">
-        <v>1025.673717893247</v>
+        <v>1025.673717892803</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>59.30719527621267</v>
+        <v>59.30719527895178</v>
       </c>
     </row>
     <row r="33">
@@ -987,16 +987,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>15134.11623427674</v>
+        <v>15134.11623430164</v>
       </c>
       <c r="C33" t="n">
-        <v>779.8838135608833</v>
+        <v>779.8838135599723</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0001159052447300504</v>
+        <v>0.0001159035878456128</v>
       </c>
       <c r="E33" t="n">
-        <v>63.74373210931567</v>
+        <v>63.74373210921021</v>
       </c>
     </row>
     <row r="34">
@@ -1004,16 +1004,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>15613.94407434368</v>
+        <v>15613.9440742929</v>
       </c>
       <c r="C34" t="n">
-        <v>799.3185131975233</v>
+        <v>799.3185132047249</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>659.0849393623649</v>
+        <v>659.0849391365837</v>
       </c>
     </row>
     <row r="35">
@@ -1021,16 +1021,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>15935.63969872032</v>
+        <v>15935.63969851564</v>
       </c>
       <c r="C35" t="n">
-        <v>649.2645952053667</v>
+        <v>649.2645953091755</v>
       </c>
       <c r="D35" t="n">
-        <v>0.095610495890248</v>
+        <v>0.09561059669684528</v>
       </c>
       <c r="E35" t="n">
-        <v>95.35436612727446</v>
+        <v>95.35436625034239</v>
       </c>
     </row>
     <row r="36">
@@ -1038,16 +1038,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>16200.60788988962</v>
+        <v>16200.60788987693</v>
       </c>
       <c r="C36" t="n">
-        <v>490.3934678884326</v>
+        <v>490.3934678879047</v>
       </c>
       <c r="D36" t="n">
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>291.0731095589169</v>
+        <v>291.0731095531051</v>
       </c>
     </row>
     <row r="37">
@@ -1055,16 +1055,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>16164.29452543894</v>
+        <v>16164.29452543333</v>
       </c>
       <c r="C37" t="n">
-        <v>487.1363820825032</v>
+        <v>487.1363820813008</v>
       </c>
       <c r="D37" t="n">
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>399.3537928355304</v>
+        <v>399.353792529083</v>
       </c>
     </row>
     <row r="38">
@@ -1072,16 +1072,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>15904.27744547573</v>
+        <v>15904.27744547181</v>
       </c>
       <c r="C38" t="n">
-        <v>574.7312931140402</v>
+        <v>574.7312931125093</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>95.21290504534925</v>
+        <v>95.21290504312859</v>
       </c>
     </row>
     <row r="39">
@@ -1089,16 +1089,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>15635.84124001202</v>
+        <v>15635.84124001076</v>
       </c>
       <c r="C39" t="n">
-        <v>731.1547170309153</v>
+        <v>731.1547170312658</v>
       </c>
       <c r="D39" t="n">
-        <v>0.004038919033515762</v>
+        <v>0.004038919927904771</v>
       </c>
       <c r="E39" t="n">
-        <v>92.00210845372196</v>
+        <v>92.00210846257264</v>
       </c>
     </row>
     <row r="40">
@@ -1106,16 +1106,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>15337.69484286975</v>
+        <v>15337.69484286773</v>
       </c>
       <c r="C40" t="n">
-        <v>835.3134968180271</v>
+        <v>835.3134968179036</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>90.78984261570936</v>
+        <v>90.78984261307079</v>
       </c>
     </row>
     <row r="41">
@@ -1123,16 +1123,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>15195.17948674785</v>
+        <v>15195.17948674502</v>
       </c>
       <c r="C41" t="n">
-        <v>898.820588040831</v>
+        <v>898.8205880412546</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>63.38886562715496</v>
+        <v>63.38886562701226</v>
       </c>
     </row>
     <row r="42">
@@ -1140,16 +1140,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>15306.27026112268</v>
+        <v>15306.2702611174</v>
       </c>
       <c r="C42" t="n">
-        <v>918.7308413482314</v>
+        <v>918.7308413481996</v>
       </c>
       <c r="D42" t="n">
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>90.68423166404079</v>
+        <v>90.68423166346167</v>
       </c>
     </row>
     <row r="43">
@@ -1157,16 +1157,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>15498.34830816019</v>
+        <v>15498.34830816136</v>
       </c>
       <c r="C43" t="n">
-        <v>1014.651166711372</v>
+        <v>1014.651166711148</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0005246038572239513</v>
+        <v>0.0005246029759544317</v>
       </c>
       <c r="E43" t="n">
-        <v>91.33374068424925</v>
+        <v>91.33374068491062</v>
       </c>
     </row>
     <row r="44">
@@ -1174,16 +1174,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>15951.34499303597</v>
+        <v>15951.3449930228</v>
       </c>
       <c r="C44" t="n">
-        <v>1050.720103032506</v>
+        <v>1050.720103032102</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>803.657078783855</v>
+        <v>803.6570786452559</v>
       </c>
     </row>
     <row r="45">
@@ -1191,16 +1191,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>15734.00793119008</v>
+        <v>15734.00793118973</v>
       </c>
       <c r="C45" t="n">
-        <v>989.991787477416</v>
+        <v>989.9917874777087</v>
       </c>
       <c r="D45" t="n">
-        <v>0.0002810515862952464</v>
+        <v>0.0002810515475682393</v>
       </c>
       <c r="E45" t="n">
-        <v>92.42334855529587</v>
+        <v>92.42334855571134</v>
       </c>
     </row>
     <row r="46">
@@ -1208,16 +1208,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>15271.77473171039</v>
+        <v>15271.77473170612</v>
       </c>
       <c r="C46" t="n">
-        <v>809.2258320796338</v>
+        <v>809.2258320793559</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>90.70631149960471</v>
+        <v>90.70631149951949</v>
       </c>
     </row>
     <row r="47">
@@ -1225,16 +1225,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>14331.27963207892</v>
+        <v>14331.27963207854</v>
       </c>
       <c r="C47" t="n">
-        <v>845.7201631186852</v>
+        <v>845.7201631189982</v>
       </c>
       <c r="D47" t="n">
-        <v>0.0002045978283864632</v>
+        <v>0.0002045979630985288</v>
       </c>
       <c r="E47" t="n">
-        <v>60.89035080201975</v>
+        <v>60.89035080150368</v>
       </c>
     </row>
     <row r="48">
@@ -1242,16 +1242,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>13102.03261779253</v>
+        <v>13102.0326177899</v>
       </c>
       <c r="C48" t="n">
-        <v>770.9697722599299</v>
+        <v>770.9697722600586</v>
       </c>
       <c r="D48" t="n">
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>59.39651643122358</v>
+        <v>59.39651643101092</v>
       </c>
     </row>
     <row r="49">
@@ -1259,16 +1259,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>11822.4429565697</v>
+        <v>11822.44295657061</v>
       </c>
       <c r="C49" t="n">
-        <v>777.5570611334381</v>
+        <v>777.5570611335929</v>
       </c>
       <c r="D49" t="n">
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>52.47977888619301</v>
+        <v>52.47977888586772</v>
       </c>
     </row>
     <row r="50">
@@ -1276,16 +1276,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>10851.05606658418</v>
+        <v>10851.05767025153</v>
       </c>
       <c r="C50" t="n">
-        <v>837.9439287303663</v>
+        <v>837.9438249550969</v>
       </c>
       <c r="D50" t="n">
-        <v>4.680788846290423e-06</v>
+        <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>29.63193651941687</v>
+        <v>29.63332407491582</v>
       </c>
     </row>
     <row r="51">
@@ -1293,16 +1293,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>10318.49307379967</v>
+        <v>10318.4930059367</v>
       </c>
       <c r="C51" t="n">
-        <v>832.506846030987</v>
+        <v>832.5068801750518</v>
       </c>
       <c r="D51" t="n">
-        <v>8.008924578574946e-05</v>
+        <v>0.0001137744864438071</v>
       </c>
       <c r="E51" t="n">
-        <v>27.34029532733151</v>
+        <v>27.33924361070935</v>
       </c>
     </row>
     <row r="52">
@@ -1310,16 +1310,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>10335.21703182314</v>
+        <v>10335.21707906758</v>
       </c>
       <c r="C52" t="n">
-        <v>518.7849413330774</v>
+        <v>518.784938127063</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
       </c>
       <c r="E52" t="n">
-        <v>27.44163838281127</v>
+        <v>27.44638735026042</v>
       </c>
     </row>
     <row r="53">
@@ -1327,16 +1327,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>10324.96594015377</v>
+        <v>10324.96599043024</v>
       </c>
       <c r="C53" t="n">
-        <v>403.0339302685526</v>
+        <v>403.0339048597881</v>
       </c>
       <c r="D53" t="n">
-        <v>0.0001294482332860842</v>
+        <v>0.0001046053696227972</v>
       </c>
       <c r="E53" t="n">
-        <v>27.37782940720233</v>
+        <v>27.37319265880775</v>
       </c>
     </row>
     <row r="54">
@@ -1344,16 +1344,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>10335.30759987077</v>
+        <v>10335.3073681142</v>
       </c>
       <c r="C54" t="n">
-        <v>469.6935678139878</v>
+        <v>469.6935830792006</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
       </c>
       <c r="E54" t="n">
-        <v>27.44103452418988</v>
+        <v>27.44163961783051</v>
       </c>
     </row>
     <row r="55">
@@ -1361,16 +1361,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>10568.10076274993</v>
+        <v>10568.10073755776</v>
       </c>
       <c r="C55" t="n">
-        <v>581.8992300793757</v>
+        <v>581.8992433411215</v>
       </c>
       <c r="D55" t="n">
-        <v>7.163528193746444e-06</v>
+        <v>1.908204375728813e-05</v>
       </c>
       <c r="E55" t="n">
-        <v>28.56057953515672</v>
+        <v>28.5608562280884</v>
       </c>
     </row>
     <row r="56">
@@ -1378,16 +1378,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>11334.26537418926</v>
+        <v>11334.2651612529</v>
       </c>
       <c r="C56" t="n">
-        <v>524.7348618485534</v>
+        <v>524.7348641011788</v>
       </c>
       <c r="D56" t="n">
-        <v>1.925071322542849e-06</v>
+        <v>4.046997193570471e-06</v>
       </c>
       <c r="E56" t="n">
-        <v>39.61451916533336</v>
+        <v>39.61452144317037</v>
       </c>
     </row>
     <row r="57">
@@ -1395,16 +1395,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>12610.39100511864</v>
+        <v>12610.37602883103</v>
       </c>
       <c r="C57" t="n">
-        <v>458.6259436396374</v>
+        <v>458.626888064324</v>
       </c>
       <c r="D57" t="n">
         <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>58.40310975416114</v>
+        <v>58.38117605941449</v>
       </c>
     </row>
     <row r="58">
@@ -1412,16 +1412,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>13700.03723868406</v>
+        <v>13700.11996808342</v>
       </c>
       <c r="C58" t="n">
-        <v>538.2043854578424</v>
+        <v>538.1887293804118</v>
       </c>
       <c r="D58" t="n">
         <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>1104.062030516781</v>
+        <v>945.9513060283447</v>
       </c>
     </row>
     <row r="59">
@@ -1429,16 +1429,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>14525.18341220254</v>
+        <v>14525.18081568391</v>
       </c>
       <c r="C59" t="n">
-        <v>476.8163822331071</v>
+        <v>476.817697729068</v>
       </c>
       <c r="D59" t="n">
-        <v>0.0002053589892449396</v>
+        <v>0.001485102038400769</v>
       </c>
       <c r="E59" t="n">
-        <v>60.48364594999777</v>
+        <v>60.44600040781216</v>
       </c>
     </row>
     <row r="60">
@@ -1446,16 +1446,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>14774.89794250277</v>
+        <v>14774.94171962412</v>
       </c>
       <c r="C60" t="n">
-        <v>461.0990163134437</v>
+        <v>461.0924282972447</v>
       </c>
       <c r="D60" t="n">
-        <v>0.003038145807882088</v>
+        <v>0</v>
       </c>
       <c r="E60" t="n">
-        <v>60.46216145485137</v>
+        <v>60.45967096650605</v>
       </c>
     </row>
     <row r="61">
@@ -1463,16 +1463,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>14776.15897853845</v>
+        <v>14776.14584916059</v>
       </c>
       <c r="C61" t="n">
-        <v>436.8472547380537</v>
+        <v>436.8510328902189</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>0.003114834528664207</v>
       </c>
       <c r="E61" t="n">
-        <v>60.41643718476904</v>
+        <v>60.43421675209039</v>
       </c>
     </row>
     <row r="62">
@@ -1480,16 +1480,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>14595.34067050063</v>
+        <v>14595.34597648899</v>
       </c>
       <c r="C62" t="n">
-        <v>354.6569363250721</v>
+        <v>354.6544573656513</v>
       </c>
       <c r="D62" t="n">
-        <v>0.002390783672541805</v>
+        <v>0</v>
       </c>
       <c r="E62" t="n">
-        <v>60.46892124601478</v>
+        <v>60.36494016283931</v>
       </c>
     </row>
     <row r="63">
@@ -1497,16 +1497,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>14383.32377211992</v>
+        <v>14383.35052308943</v>
       </c>
       <c r="C63" t="n">
-        <v>242.6742206870197</v>
+        <v>242.6702674190358</v>
       </c>
       <c r="D63" t="n">
-        <v>0.002005187987065038</v>
+        <v>0</v>
       </c>
       <c r="E63" t="n">
-        <v>59.67777430503087</v>
+        <v>59.79689760393416</v>
       </c>
     </row>
     <row r="64">
@@ -1514,16 +1514,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>14156.66597893773</v>
+        <v>14156.65590869122</v>
       </c>
       <c r="C64" t="n">
-        <v>194.3404388572625</v>
+        <v>194.3425579031849</v>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>0.001531873781050039</v>
       </c>
       <c r="E64" t="n">
-        <v>59.22497583871032</v>
+        <v>59.21190945382736</v>
       </c>
     </row>
     <row r="65">
@@ -1531,16 +1531,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>14066.24093271521</v>
+        <v>14066.21240113039</v>
       </c>
       <c r="C65" t="n">
-        <v>167.7941242315286</v>
+        <v>167.7965095506964</v>
       </c>
       <c r="D65" t="n">
         <v>0</v>
       </c>
       <c r="E65" t="n">
-        <v>59.03511022019391</v>
+        <v>59.06515857852767</v>
       </c>
     </row>
     <row r="66">
@@ -1548,16 +1548,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>14264.1317596381</v>
+        <v>14264.13383885605</v>
       </c>
       <c r="C66" t="n">
-        <v>217.8664873616794</v>
+        <v>217.8654369329095</v>
       </c>
       <c r="D66" t="n">
-        <v>0.001751249048453722</v>
+        <v>0.0007234875829401684</v>
       </c>
       <c r="E66" t="n">
-        <v>59.56234479414107</v>
+        <v>59.46023074147152</v>
       </c>
     </row>
     <row r="67">
@@ -1565,16 +1565,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>14585.74808109017</v>
+        <v>14585.76138113063</v>
       </c>
       <c r="C67" t="n">
-        <v>398.2501330369728</v>
+        <v>398.2474885804104</v>
       </c>
       <c r="D67" t="n">
-        <v>0.001784088917447845</v>
+        <v>0</v>
       </c>
       <c r="E67" t="n">
-        <v>60.4386331780405</v>
+        <v>60.38646072171679</v>
       </c>
     </row>
     <row r="68">
@@ -1582,16 +1582,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>14761.53789691745</v>
+        <v>14761.54210779619</v>
       </c>
       <c r="C68" t="n">
-        <v>870.2122707351871</v>
+        <v>870.2120389045803</v>
       </c>
       <c r="D68" t="n">
         <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>281.6270034474296</v>
+        <v>274.4192282684584</v>
       </c>
     </row>
     <row r="69">
@@ -1599,16 +1599,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>14300.00829549922</v>
+        <v>14300.01158313267</v>
       </c>
       <c r="C69" t="n">
-        <v>1194.62951805316</v>
+        <v>1194.629381012152</v>
       </c>
       <c r="D69" t="n">
         <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>578.7196949992258</v>
+        <v>574.2561665421696</v>
       </c>
     </row>
     <row r="70">
@@ -1616,16 +1616,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>13608.13409314558</v>
+        <v>13608.13625547324</v>
       </c>
       <c r="C70" t="n">
-        <v>1360.894711653705</v>
+        <v>1360.894137813196</v>
       </c>
       <c r="D70" t="n">
-        <v>0.0005266978202899973</v>
+        <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>59.4791980873832</v>
+        <v>59.47147917787076</v>
       </c>
     </row>
     <row r="71">
@@ -1633,16 +1633,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>12729.50201778181</v>
+        <v>12729.50225824897</v>
       </c>
       <c r="C71" t="n">
-        <v>1468.497841490951</v>
+        <v>1468.497720934525</v>
       </c>
       <c r="D71" t="n">
-        <v>0.000140586674799286</v>
+        <v>2.295108463164541e-05</v>
       </c>
       <c r="E71" t="n">
-        <v>58.9267772983678</v>
+        <v>58.92413045744078</v>
       </c>
     </row>
     <row r="72">
@@ -1650,16 +1650,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>11667.11903668195</v>
+        <v>11667.12135366811</v>
       </c>
       <c r="C72" t="n">
-        <v>1511.88083599602</v>
+        <v>1511.880572529431</v>
       </c>
       <c r="D72" t="n">
-        <v>0.0001271948475758654</v>
+        <v>0</v>
       </c>
       <c r="E72" t="n">
-        <v>52.04272803423403</v>
+        <v>52.03763177924985</v>
       </c>
     </row>
     <row r="73">
@@ -1667,16 +1667,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>10942.50099082665</v>
+        <v>10942.50095512549</v>
       </c>
       <c r="C73" t="n">
-        <v>1176.499098229465</v>
+        <v>1176.499100576739</v>
       </c>
       <c r="D73" t="n">
         <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>30.09864181233023</v>
+        <v>30.09887787050564</v>
       </c>
     </row>
     <row r="74">
@@ -1684,16 +1684,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>10347.55796912205</v>
+        <v>10347.55796914651</v>
       </c>
       <c r="C74" t="n">
-        <v>849.4432206670714</v>
+        <v>849.4432206655717</v>
       </c>
       <c r="D74" t="n">
         <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>27.79707299216761</v>
+        <v>27.79707298906251</v>
       </c>
     </row>
     <row r="75">
@@ -1701,16 +1701,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>9560.453256724964</v>
+        <v>9560.453256724943</v>
       </c>
       <c r="C75" t="n">
-        <v>708.5467436753268</v>
+        <v>708.54674367537</v>
       </c>
       <c r="D75" t="n">
         <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>25.91834099137916</v>
+        <v>25.91834099096486</v>
       </c>
     </row>
     <row r="76">
@@ -1718,16 +1718,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>10057.85867845695</v>
+        <v>10057.8586784553</v>
       </c>
       <c r="C76" t="n">
-        <v>553.1413258099406</v>
+        <v>553.1413258100627</v>
       </c>
       <c r="D76" t="n">
         <v>0</v>
       </c>
       <c r="E76" t="n">
-        <v>26.9578890049557</v>
+        <v>26.95788900310007</v>
       </c>
     </row>
     <row r="77">
@@ -1735,16 +1735,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>9909.279703125736</v>
+        <v>9909.279703124872</v>
       </c>
       <c r="C77" t="n">
-        <v>416.7203017289837</v>
+        <v>416.7203017290842</v>
       </c>
       <c r="D77" t="n">
         <v>0</v>
       </c>
       <c r="E77" t="n">
-        <v>26.59690547243997</v>
+        <v>26.59690547358873</v>
       </c>
     </row>
     <row r="78">
@@ -1752,16 +1752,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>9804.27500155706</v>
+        <v>9804.275001557142</v>
       </c>
       <c r="C78" t="n">
-        <v>457.7249983309421</v>
+        <v>457.7249983309521</v>
       </c>
       <c r="D78" t="n">
-        <v>1.691652764814254e-07</v>
+        <v>1.69104497011e-07</v>
       </c>
       <c r="E78" t="n">
-        <v>26.37566819130086</v>
+        <v>26.37566819061872</v>
       </c>
     </row>
     <row r="79">
@@ -1769,16 +1769,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>9857.855623119325</v>
+        <v>9857.855623119531</v>
       </c>
       <c r="C79" t="n">
-        <v>523.144376538613</v>
+        <v>523.1443765384785</v>
       </c>
       <c r="D79" t="n">
-        <v>3.417237892904248e-07</v>
+        <v>3.416358456591656e-07</v>
       </c>
       <c r="E79" t="n">
-        <v>26.48856719216667</v>
+        <v>26.4885671917478</v>
       </c>
     </row>
     <row r="80">
@@ -1786,16 +1786,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>10125.8884129681</v>
+        <v>10125.88841296647</v>
       </c>
       <c r="C80" t="n">
-        <v>551.1115953276123</v>
+        <v>551.1115953275998</v>
       </c>
       <c r="D80" t="n">
         <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>27.15719005440351</v>
+        <v>27.15719005409977</v>
       </c>
     </row>
     <row r="81">
@@ -1803,16 +1803,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>10660.52353813436</v>
+        <v>10660.52353813369</v>
       </c>
       <c r="C81" t="n">
-        <v>513.4764517605888</v>
+        <v>513.4764517608564</v>
       </c>
       <c r="D81" t="n">
-        <v>1.009496056171178e-05</v>
+        <v>1.009533009183155e-05</v>
       </c>
       <c r="E81" t="n">
-        <v>28.97402374837301</v>
+        <v>28.97402374525482</v>
       </c>
     </row>
     <row r="82">
@@ -1820,16 +1820,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>11527.57964290493</v>
+        <v>11527.57964261754</v>
       </c>
       <c r="C82" t="n">
-        <v>531.9998352531725</v>
+        <v>531.9998352640717</v>
       </c>
       <c r="D82" t="n">
         <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>1845.742743771107</v>
+        <v>1845.742895221974</v>
       </c>
     </row>
     <row r="83">
@@ -1837,16 +1837,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>12621.39476380882</v>
+        <v>12621.3947637937</v>
       </c>
       <c r="C83" t="n">
-        <v>333.6050603321866</v>
+        <v>333.6050603396499</v>
       </c>
       <c r="D83" t="n">
-        <v>0.0001756833488947273</v>
+        <v>0.0001756910326374963</v>
       </c>
       <c r="E83" t="n">
-        <v>58.49647160359797</v>
+        <v>58.4964716043194</v>
       </c>
     </row>
     <row r="84">
@@ -1854,16 +1854,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>13290.37103409272</v>
+        <v>13290.37103391168</v>
       </c>
       <c r="C84" t="n">
-        <v>304.2011775337979</v>
+        <v>304.2011775424867</v>
       </c>
       <c r="D84" t="n">
         <v>0</v>
       </c>
       <c r="E84" t="n">
-        <v>1288.414323017858</v>
+        <v>1288.41449166153</v>
       </c>
     </row>
     <row r="85">
@@ -1871,16 +1871,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>13651.84903523786</v>
+        <v>13651.84903498225</v>
       </c>
       <c r="C85" t="n">
-        <v>310.1483799019917</v>
+        <v>310.1483800318418</v>
       </c>
       <c r="D85" t="n">
-        <v>0.002582278585087679</v>
+        <v>0.002582404241806898</v>
       </c>
       <c r="E85" t="n">
-        <v>59.68796352880606</v>
+        <v>59.68796394555917</v>
       </c>
     </row>
     <row r="86">
@@ -1888,16 +1888,16 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>13754.10888513868</v>
+        <v>13754.10888524978</v>
       </c>
       <c r="C86" t="n">
-        <v>347.6087009599844</v>
+        <v>347.6087009560222</v>
       </c>
       <c r="D86" t="n">
         <v>0</v>
       </c>
       <c r="E86" t="n">
-        <v>316.8130527248792</v>
+        <v>316.8132824035461</v>
       </c>
     </row>
     <row r="87">
@@ -1905,16 +1905,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>13628.98996000322</v>
+        <v>13628.98996241549</v>
       </c>
       <c r="C87" t="n">
-        <v>415.0276153471602</v>
+        <v>415.0276151660958</v>
       </c>
       <c r="D87" t="n">
         <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>59.65220740948939</v>
+        <v>59.65220735495148</v>
       </c>
     </row>
     <row r="88">
@@ -1922,16 +1922,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>13450.20334201867</v>
+        <v>13450.20334226768</v>
       </c>
       <c r="C88" t="n">
-        <v>446.7951387550556</v>
+        <v>446.7951386283694</v>
       </c>
       <c r="D88" t="n">
-        <v>0.001517708710438851</v>
+        <v>0.001517586522839705</v>
       </c>
       <c r="E88" t="n">
-        <v>59.22891251783943</v>
+        <v>59.22891211038407</v>
       </c>
     </row>
     <row r="89">
@@ -1939,16 +1939,16 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>13515.95152849347</v>
+        <v>13515.9515283594</v>
       </c>
       <c r="C89" t="n">
-        <v>302.0881859553413</v>
+        <v>302.0881859695309</v>
       </c>
       <c r="D89" t="n">
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>59.39116273765996</v>
+        <v>59.39116304778425</v>
       </c>
     </row>
     <row r="90">
@@ -1956,16 +1956,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>13786.91782877385</v>
+        <v>13786.91782824771</v>
       </c>
       <c r="C90" t="n">
-        <v>257.0802162235374</v>
+        <v>257.0802164840593</v>
       </c>
       <c r="D90" t="n">
-        <v>0.001953050549652789</v>
+        <v>0.001953315913355181</v>
       </c>
       <c r="E90" t="n">
-        <v>59.38123160985123</v>
+        <v>59.38123178856149</v>
       </c>
     </row>
     <row r="91">
@@ -1973,16 +1973,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>14003.55094429376</v>
+        <v>14003.55094424681</v>
       </c>
       <c r="C91" t="n">
-        <v>531.446781443542</v>
+        <v>531.4467814674288</v>
       </c>
       <c r="D91" t="n">
-        <v>0.002271993764188854</v>
+        <v>0.0022720168316099</v>
       </c>
       <c r="E91" t="n">
-        <v>59.62096542283675</v>
+        <v>59.62096469831121</v>
       </c>
     </row>
     <row r="92">
@@ -1990,16 +1990,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>14290.38052223557</v>
+        <v>14290.3805245818</v>
       </c>
       <c r="C92" t="n">
-        <v>706.6334091767555</v>
+        <v>706.6334089231909</v>
       </c>
       <c r="D92" t="n">
         <v>0</v>
       </c>
       <c r="E92" t="n">
-        <v>59.98883766134046</v>
+        <v>59.98883849384218</v>
       </c>
     </row>
     <row r="93">
@@ -2007,16 +2007,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>14814.70952001754</v>
+        <v>14814.70952055872</v>
       </c>
       <c r="C93" t="n">
-        <v>819.3187580870742</v>
+        <v>819.3187580703427</v>
       </c>
       <c r="D93" t="n">
         <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>986.494125716722</v>
+        <v>986.4941429784358</v>
       </c>
     </row>
     <row r="94">
@@ -2024,16 +2024,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>14723.44215716369</v>
+        <v>14723.44215575743</v>
       </c>
       <c r="C94" t="n">
-        <v>834.7429871374131</v>
+        <v>834.742987233248</v>
       </c>
       <c r="D94" t="n">
         <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>535.9800034958622</v>
+        <v>535.980109920658</v>
       </c>
     </row>
     <row r="95">
@@ -2041,16 +2041,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>13952.1417570839</v>
+        <v>13952.14175463034</v>
       </c>
       <c r="C95" t="n">
-        <v>697.8254774792242</v>
+        <v>697.8254787069327</v>
       </c>
       <c r="D95" t="n">
-        <v>0.03273271063588645</v>
+        <v>0.03273393522761853</v>
       </c>
       <c r="E95" t="n">
-        <v>60.22652645230287</v>
+        <v>60.22653347822053</v>
       </c>
     </row>
     <row r="96">
@@ -2058,16 +2058,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>12811.76217061049</v>
+        <v>12811.76216471459</v>
       </c>
       <c r="C96" t="n">
-        <v>658.3151108546967</v>
+        <v>658.3151112871763</v>
       </c>
       <c r="D96" t="n">
         <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>59.24045144724826</v>
+        <v>59.24045503478381</v>
       </c>
     </row>
     <row r="97">
@@ -2075,16 +2075,16 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>11553.4083896902</v>
+        <v>11553.40838971796</v>
       </c>
       <c r="C97" t="n">
-        <v>724.5911019789834</v>
+        <v>724.5911019601538</v>
       </c>
       <c r="D97" t="n">
-        <v>0.0005078227716128585</v>
+        <v>0.0005078138388384313</v>
       </c>
       <c r="E97" t="n">
-        <v>51.56370189057599</v>
+        <v>51.56370184774084</v>
       </c>
     </row>
     <row r="98">
@@ -2092,16 +2092,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>11014.18070729601</v>
+        <v>11014.18070729585</v>
       </c>
       <c r="C98" t="n">
-        <v>669.8183960523883</v>
+        <v>669.8183960523734</v>
       </c>
       <c r="D98" t="n">
-        <v>0.0008957560352167006</v>
+        <v>0.0008957561775915681</v>
       </c>
       <c r="E98" t="n">
-        <v>30.55936716329964</v>
+        <v>30.55936716320917</v>
       </c>
     </row>
     <row r="99">
@@ -2109,16 +2109,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>10540.56410570881</v>
+        <v>10540.56410570914</v>
       </c>
       <c r="C99" t="n">
-        <v>673.4452522087822</v>
+        <v>673.4452522088095</v>
       </c>
       <c r="D99" t="n">
         <v>0</v>
       </c>
       <c r="E99" t="n">
-        <v>28.48329024482296</v>
+        <v>28.48329024418829</v>
       </c>
     </row>
     <row r="100">
@@ -2126,16 +2126,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>10476.7078157699</v>
+        <v>10476.70781576981</v>
       </c>
       <c r="C100" t="n">
-        <v>523.2834865006071</v>
+        <v>523.2834865005551</v>
       </c>
       <c r="D100" t="n">
-        <v>0.00868904170971645</v>
+        <v>0.008689041824105525</v>
       </c>
       <c r="E100" t="n">
-        <v>28.26197567487138</v>
+        <v>28.26197567645833</v>
       </c>
     </row>
     <row r="101">
@@ -2143,16 +2143,16 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>10607.37661213817</v>
+        <v>10607.3766121379</v>
       </c>
       <c r="C101" t="n">
-        <v>333.6228816256342</v>
+        <v>333.6228816257955</v>
       </c>
       <c r="D101" t="n">
-        <v>0.0005057307511281571</v>
+        <v>0.0005057308943962745</v>
       </c>
       <c r="E101" t="n">
-        <v>28.67291768429106</v>
+        <v>28.67291768406443</v>
       </c>
     </row>
     <row r="102">
@@ -2160,16 +2160,16 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>10870.3420204793</v>
+        <v>10870.34202047967</v>
       </c>
       <c r="C102" t="n">
-        <v>368.7424208353117</v>
+        <v>368.7424208352987</v>
       </c>
       <c r="D102" t="n">
         <v>0</v>
       </c>
       <c r="E102" t="n">
-        <v>29.74766058815015</v>
+        <v>29.74766058887365</v>
       </c>
     </row>
     <row r="103">
@@ -2177,16 +2177,16 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>11902.38534008094</v>
+        <v>11902.3853400817</v>
       </c>
       <c r="C103" t="n">
-        <v>434.7619802101927</v>
+        <v>434.7619802100659</v>
       </c>
       <c r="D103" t="n">
         <v>0</v>
       </c>
       <c r="E103" t="n">
-        <v>52.82433950648242</v>
+        <v>52.82433950659833</v>
       </c>
     </row>
     <row r="104">
@@ -2194,16 +2194,16 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>13885.69270528265</v>
+        <v>13885.69270528145</v>
       </c>
       <c r="C104" t="n">
-        <v>457.328500918459</v>
+        <v>457.3285009186414</v>
       </c>
       <c r="D104" t="n">
         <v>0</v>
       </c>
       <c r="E104" t="n">
-        <v>1045.569231970939</v>
+        <v>1045.569231981699</v>
       </c>
     </row>
     <row r="105">
@@ -2211,16 +2211,16 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>15478.31396968846</v>
+        <v>15478.31396968859</v>
       </c>
       <c r="C105" t="n">
-        <v>435.6827613813677</v>
+        <v>435.6827613814472</v>
       </c>
       <c r="D105" t="n">
-        <v>0.003265664742042448</v>
+        <v>0.003265664610053372</v>
       </c>
       <c r="E105" t="n">
-        <v>91.46863930827649</v>
+        <v>91.46863930778404</v>
       </c>
     </row>
     <row r="106">
@@ -2228,16 +2228,16 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>16088.83273445771</v>
+        <v>16088.8327344588</v>
       </c>
       <c r="C106" t="n">
-        <v>324.6905420577822</v>
+        <v>324.6905420575741</v>
       </c>
       <c r="D106" t="n">
         <v>0</v>
       </c>
       <c r="E106" t="n">
-        <v>336.3318698852248</v>
+        <v>336.3318698826028</v>
       </c>
     </row>
     <row r="107">
@@ -2245,16 +2245,16 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>16320.37097754435</v>
+        <v>16320.37097754414</v>
       </c>
       <c r="C107" t="n">
-        <v>264.6290182344947</v>
+        <v>264.629018234518</v>
       </c>
       <c r="D107" t="n">
-        <v>4.216964748665072e-06</v>
+        <v>4.217137397156827e-06</v>
       </c>
       <c r="E107" t="n">
-        <v>158.7015114727039</v>
+        <v>158.7015114716566</v>
       </c>
     </row>
     <row r="108">
@@ -2262,16 +2262,16 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>16448.602744641</v>
+        <v>16448.60274464044</v>
       </c>
       <c r="C108" t="n">
-        <v>242.3962475206049</v>
+        <v>242.3962475207404</v>
       </c>
       <c r="D108" t="n">
-        <v>0.001006831629013816</v>
+        <v>0.001006832085217373</v>
       </c>
       <c r="E108" t="n">
-        <v>290.367655519844</v>
+        <v>290.3676555167705</v>
       </c>
     </row>
     <row r="109">
@@ -2279,16 +2279,16 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>16422.25462176661</v>
+        <v>16422.25462176734</v>
       </c>
       <c r="C109" t="n">
-        <v>229.3424901309776</v>
+        <v>229.3424901308368</v>
       </c>
       <c r="D109" t="n">
         <v>0</v>
       </c>
       <c r="E109" t="n">
-        <v>177.2562005737711</v>
+        <v>177.2562005688191</v>
       </c>
     </row>
     <row r="110">
@@ -2296,16 +2296,16 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>16260.82385432638</v>
+        <v>16260.82385432673</v>
       </c>
       <c r="C110" t="n">
-        <v>218.6239440461079</v>
+        <v>218.6239440460087</v>
       </c>
       <c r="D110" t="n">
         <v>0</v>
       </c>
       <c r="E110" t="n">
-        <v>375.8779873234417</v>
+        <v>375.8779873246956</v>
       </c>
     </row>
     <row r="111">
@@ -2313,16 +2313,16 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>16158.6283730623</v>
+        <v>16158.62837306235</v>
       </c>
       <c r="C111" t="n">
-        <v>208.588891770071</v>
+        <v>208.5888917700807</v>
       </c>
       <c r="D111" t="n">
         <v>0</v>
       </c>
       <c r="E111" t="n">
-        <v>648.248609022294</v>
+        <v>648.2486090283231</v>
       </c>
     </row>
     <row r="112">
@@ -2330,16 +2330,16 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>15946.47695862145</v>
+        <v>15946.47695862215</v>
       </c>
       <c r="C112" t="n">
-        <v>226.9266424391328</v>
+        <v>226.9266424393165</v>
       </c>
       <c r="D112" t="n">
         <v>0</v>
       </c>
       <c r="E112" t="n">
-        <v>491.441856025208</v>
+        <v>491.4418560272344</v>
       </c>
     </row>
     <row r="113">
@@ -2347,16 +2347,16 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>15873.43637319954</v>
+        <v>15873.4363731983</v>
       </c>
       <c r="C113" t="n">
-        <v>220.5880414697183</v>
+        <v>220.5880414695716</v>
       </c>
       <c r="D113" t="n">
         <v>0</v>
       </c>
       <c r="E113" t="n">
-        <v>92.87847182001487</v>
+        <v>92.87847182004229</v>
       </c>
     </row>
     <row r="114">
@@ -2364,16 +2364,16 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>15926.58409922548</v>
+        <v>15926.58409922518</v>
       </c>
       <c r="C114" t="n">
-        <v>298.9178562597425</v>
+        <v>298.9178562596193</v>
       </c>
       <c r="D114" t="n">
         <v>0</v>
       </c>
       <c r="E114" t="n">
-        <v>536.7816982082246</v>
+        <v>536.7816982119659</v>
       </c>
     </row>
     <row r="115">
@@ -2381,16 +2381,16 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>16012.55123804215</v>
+        <v>16012.55123804127</v>
       </c>
       <c r="C115" t="n">
-        <v>500.9053427654202</v>
+        <v>500.9053427653611</v>
       </c>
       <c r="D115" t="n">
         <v>0</v>
       </c>
       <c r="E115" t="n">
-        <v>497.9302891690963</v>
+        <v>497.9302891733075</v>
       </c>
     </row>
     <row r="116">
@@ -2398,16 +2398,16 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>16561.70551509326</v>
+        <v>16561.70551509248</v>
       </c>
       <c r="C116" t="n">
-        <v>440.5729538791771</v>
+        <v>440.5729538789878</v>
       </c>
       <c r="D116" t="n">
         <v>0</v>
       </c>
       <c r="E116" t="n">
-        <v>645.3488161396235</v>
+        <v>645.3488161424618</v>
       </c>
     </row>
     <row r="117">
@@ -2415,16 +2415,16 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>16438.46737039229</v>
+        <v>16438.46737039167</v>
       </c>
       <c r="C117" t="n">
-        <v>285.5909398468308</v>
+        <v>285.5909398470922</v>
       </c>
       <c r="D117" t="n">
         <v>0</v>
       </c>
       <c r="E117" t="n">
-        <v>296.6176495270974</v>
+        <v>296.6176495282439</v>
       </c>
     </row>
     <row r="118">
@@ -2432,16 +2432,16 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>15925.23256636305</v>
+        <v>15925.23256636363</v>
       </c>
       <c r="C118" t="n">
-        <v>155.8906674430418</v>
+        <v>155.890667443132</v>
       </c>
       <c r="D118" t="n">
         <v>0</v>
       </c>
       <c r="E118" t="n">
-        <v>95.4462806084854</v>
+        <v>95.44628060806406</v>
       </c>
     </row>
     <row r="119">
@@ -2449,16 +2449,16 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>15046.97102493745</v>
+        <v>15046.97102493706</v>
       </c>
       <c r="C119" t="n">
-        <v>130.0295266461011</v>
+        <v>130.0295266462121</v>
       </c>
       <c r="D119" t="n">
-        <v>0.000423200217384768</v>
+        <v>0.0004232002505662287</v>
       </c>
       <c r="E119" t="n">
-        <v>63.08677325567934</v>
+        <v>63.08677325530083</v>
       </c>
     </row>
     <row r="120">
@@ -2466,16 +2466,16 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>13780.92808156249</v>
+        <v>13780.92808156282</v>
       </c>
       <c r="C120" t="n">
-        <v>92.07135751572713</v>
+        <v>92.07135751559923</v>
       </c>
       <c r="D120" t="n">
-        <v>0.0005603613978752821</v>
+        <v>0.0005603612000251623</v>
       </c>
       <c r="E120" t="n">
-        <v>59.88610629833007</v>
+        <v>59.88610629838428</v>
       </c>
     </row>
     <row r="121">
@@ -2483,16 +2483,16 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>12507.54907955694</v>
+        <v>12507.5490795557</v>
       </c>
       <c r="C121" t="n">
-        <v>92.46067584735869</v>
+        <v>92.46067584731732</v>
       </c>
       <c r="D121" t="n">
         <v>0</v>
       </c>
       <c r="E121" t="n">
-        <v>59.51322285251346</v>
+        <v>59.51322285310864</v>
       </c>
     </row>
     <row r="122">
@@ -2500,16 +2500,16 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>11598.22909372732</v>
+        <v>11598.2106878126</v>
       </c>
       <c r="C122" t="n">
-        <v>90.79448620354241</v>
+        <v>90.79565258560484</v>
       </c>
       <c r="D122" t="n">
         <v>0</v>
       </c>
       <c r="E122" t="n">
-        <v>57.84578007631659</v>
+        <v>57.87951740105829</v>
       </c>
     </row>
     <row r="123">
@@ -2517,16 +2517,16 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>11044.9588312373</v>
+        <v>11044.93187895324</v>
       </c>
       <c r="C123" t="n">
-        <v>106.0724880051566</v>
+        <v>106.074200841556</v>
       </c>
       <c r="D123" t="n">
         <v>0</v>
       </c>
       <c r="E123" t="n">
-        <v>30.00489932534109</v>
+        <v>29.97152318626596</v>
       </c>
     </row>
     <row r="124">
@@ -2534,16 +2534,16 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>10824.58165270229</v>
+        <v>10824.57946791948</v>
       </c>
       <c r="C124" t="n">
-        <v>29.42844362007643</v>
+        <v>29.42858295202233</v>
       </c>
       <c r="D124" t="n">
         <v>0</v>
       </c>
       <c r="E124" t="n">
-        <v>28.92439919814356</v>
+        <v>28.93250688279091</v>
       </c>
     </row>
     <row r="125">
@@ -2551,16 +2551,16 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>10727.99761170583</v>
+        <v>10727.99847552822</v>
       </c>
       <c r="C125" t="n">
-        <v>0.0007951414566131723</v>
+        <v>0.0005076047054595259</v>
       </c>
       <c r="D125" t="n">
-        <v>0.001591561237506129</v>
+        <v>0.001015851250493615</v>
       </c>
       <c r="E125" t="n">
-        <v>28.63415318884634</v>
+        <v>28.642659009875</v>
       </c>
     </row>
     <row r="126">
@@ -2568,7 +2568,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>10805.01476886258</v>
+        <v>10805.01477151377</v>
       </c>
       <c r="C126" t="n">
         <v>0</v>
@@ -2577,7 +2577,7 @@
         <v>0</v>
       </c>
       <c r="E126" t="n">
-        <v>28.87041511200731</v>
+        <v>28.86822525445389</v>
       </c>
     </row>
     <row r="127">
@@ -2585,16 +2585,16 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>11149.99976186333</v>
+        <v>11149.99937972694</v>
       </c>
       <c r="C127" t="n">
-        <v>7.935519198344656e-05</v>
+        <v>0.0002067153447923466</v>
       </c>
       <c r="D127" t="n">
-        <v>0.0001586228752946622</v>
+        <v>0.0004131445974145158</v>
       </c>
       <c r="E127" t="n">
-        <v>30.5686231850073</v>
+        <v>30.57288122967343</v>
       </c>
     </row>
     <row r="128">
@@ -2602,16 +2602,16 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>11858.99927488951</v>
+        <v>11858.99966838719</v>
       </c>
       <c r="C128" t="n">
-        <v>0.0002409590513656609</v>
+        <v>0.0001102148707741673</v>
       </c>
       <c r="D128" t="n">
-        <v>0.0004836678348832031</v>
+        <v>0.0002211767690606975</v>
       </c>
       <c r="E128" t="n">
-        <v>52.53998763712373</v>
+        <v>52.5373550209733</v>
       </c>
     </row>
     <row r="129">
@@ -2619,7 +2619,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>13069.38076404673</v>
+        <v>13069.38376829874</v>
       </c>
       <c r="C129" t="n">
         <v>0</v>
@@ -2628,7 +2628,7 @@
         <v>0</v>
       </c>
       <c r="E129" t="n">
-        <v>1334.959397654528</v>
+        <v>1294.716682436825</v>
       </c>
     </row>
     <row r="130">
@@ -2636,7 +2636,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>14238.00060215413</v>
+        <v>14238.00030039985</v>
       </c>
       <c r="C130" t="n">
         <v>0</v>
@@ -2645,7 +2645,7 @@
         <v>0</v>
       </c>
       <c r="E130" t="n">
-        <v>60.24060721195907</v>
+        <v>60.24225564625036</v>
       </c>
     </row>
     <row r="131">
@@ -2653,7 +2653,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>15002.00012408949</v>
+        <v>15002.00003466737</v>
       </c>
       <c r="C131" t="n">
         <v>0</v>
@@ -2662,7 +2662,7 @@
         <v>0</v>
       </c>
       <c r="E131" t="n">
-        <v>90.70488024106427</v>
+        <v>90.7129054270123</v>
       </c>
     </row>
     <row r="132">
@@ -2670,16 +2670,16 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>15235.99987102812</v>
+        <v>15236.00016471554</v>
       </c>
       <c r="C132" t="n">
-        <v>4.238918931785487e-05</v>
+        <v>0</v>
       </c>
       <c r="D132" t="n">
-        <v>8.649619094101955e-05</v>
+        <v>0</v>
       </c>
       <c r="E132" t="n">
-        <v>90.85478331424031</v>
+        <v>90.85584162352818</v>
       </c>
     </row>
     <row r="133">
@@ -2687,16 +2687,16 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>15213.00064448355</v>
+        <v>15212.99998719686</v>
       </c>
       <c r="C133" t="n">
-        <v>0</v>
+        <v>4.746587390011463e-06</v>
       </c>
       <c r="D133" t="n">
-        <v>0</v>
+        <v>8.048520375132191e-06</v>
       </c>
       <c r="E133" t="n">
-        <v>90.8127967568619</v>
+        <v>90.81451931648954</v>
       </c>
     </row>
     <row r="134">
@@ -2704,16 +2704,16 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>14949.99963682692</v>
+        <v>14950.00244016137</v>
       </c>
       <c r="C134" t="n">
-        <v>0.0001210210987427772</v>
+        <v>0</v>
       </c>
       <c r="D134" t="n">
-        <v>0.0002419100768744234</v>
+        <v>0</v>
       </c>
       <c r="E134" t="n">
-        <v>90.29591863157556</v>
+        <v>90.29473100341714</v>
       </c>
     </row>
     <row r="135">
@@ -2721,16 +2721,16 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>14625.9999917887</v>
+        <v>14625.99999355647</v>
       </c>
       <c r="C135" t="n">
-        <v>2.739995980703877e-06</v>
+        <v>2.151211021489989e-06</v>
       </c>
       <c r="D135" t="n">
-        <v>5.46583653680289e-06</v>
+        <v>4.288041073590659e-06</v>
       </c>
       <c r="E135" t="n">
-        <v>60.23401783091965</v>
+        <v>60.23480294847998</v>
       </c>
     </row>
     <row r="136">
@@ -2738,7 +2738,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>14351.00016788998</v>
+        <v>14351.00007062863</v>
       </c>
       <c r="C136" t="n">
         <v>0</v>
@@ -2747,7 +2747,7 @@
         <v>0</v>
       </c>
       <c r="E136" t="n">
-        <v>59.49535988032655</v>
+        <v>59.49532268956506</v>
       </c>
     </row>
     <row r="137">
@@ -2755,16 +2755,16 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>14233.99998308038</v>
+        <v>14234.00000009385</v>
       </c>
       <c r="C137" t="n">
-        <v>5.6571087355931e-06</v>
+        <v>0</v>
       </c>
       <c r="D137" t="n">
-        <v>1.125127469480921e-05</v>
+        <v>0</v>
       </c>
       <c r="E137" t="n">
-        <v>59.20439857655887</v>
+        <v>59.20474779388233</v>
       </c>
     </row>
     <row r="138">
@@ -2772,16 +2772,16 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>14456.55872416418</v>
+        <v>14456.55859067469</v>
       </c>
       <c r="C138" t="n">
-        <v>25.44145811070359</v>
+        <v>25.44146988367561</v>
       </c>
       <c r="D138" t="n">
         <v>0</v>
       </c>
       <c r="E138" t="n">
-        <v>59.74784160609168</v>
+        <v>59.74796129871784</v>
       </c>
     </row>
     <row r="139">
@@ -2789,16 +2789,16 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>14895.29167695375</v>
+        <v>14895.29163999857</v>
       </c>
       <c r="C139" t="n">
-        <v>88.70827155306263</v>
+        <v>88.70829013611535</v>
       </c>
       <c r="D139" t="n">
-        <v>5.144175215608257e-05</v>
+        <v>6.979551623217566e-05</v>
       </c>
       <c r="E139" t="n">
-        <v>61.97624107752847</v>
+        <v>61.97542596004307</v>
       </c>
     </row>
     <row r="140">
@@ -2806,16 +2806,16 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>15406.33360144358</v>
+        <v>15406.33418240684</v>
       </c>
       <c r="C140" t="n">
-        <v>224.6634218173907</v>
+        <v>224.6631332481644</v>
       </c>
       <c r="D140" t="n">
-        <v>0.002973765361099709</v>
+        <v>0.002681663435190606</v>
       </c>
       <c r="E140" t="n">
-        <v>91.38625493018772</v>
+        <v>91.31957450363069</v>
       </c>
     </row>
     <row r="141">
@@ -2823,16 +2823,16 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>15196.57331673217</v>
+        <v>15196.57085022654</v>
       </c>
       <c r="C141" t="n">
-        <v>297.4547229103443</v>
+        <v>297.456302741533</v>
       </c>
       <c r="D141" t="n">
         <v>0</v>
       </c>
       <c r="E141" t="n">
-        <v>90.79120981551134</v>
+        <v>90.91818607760537</v>
       </c>
     </row>
     <row r="142">
@@ -2840,16 +2840,16 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>14687.65372442762</v>
+        <v>14687.65368739125</v>
       </c>
       <c r="C142" t="n">
-        <v>281.3462343525907</v>
+        <v>281.3462529226655</v>
       </c>
       <c r="D142" t="n">
-        <v>4.117862496576594e-05</v>
+        <v>5.962646994382822e-05</v>
       </c>
       <c r="E142" t="n">
-        <v>60.98225027349545</v>
+        <v>60.98468564759773</v>
       </c>
     </row>
     <row r="143">
@@ -2857,16 +2857,16 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>13905.42871895343</v>
+        <v>13905.42877463187</v>
       </c>
       <c r="C143" t="n">
-        <v>292.5712334917708</v>
+        <v>292.571456705203</v>
       </c>
       <c r="D143" t="n">
-        <v>0.0004647909598109914</v>
+        <v>0.000686504974364685</v>
       </c>
       <c r="E143" t="n">
-        <v>60.65259278768878</v>
+        <v>60.65444932567621</v>
       </c>
     </row>
     <row r="144">
@@ -2874,16 +2874,16 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>12915.40599134341</v>
+        <v>12915.39900409773</v>
       </c>
       <c r="C144" t="n">
-        <v>263.6097059338836</v>
+        <v>263.610192949334</v>
       </c>
       <c r="D144" t="n">
         <v>0</v>
       </c>
       <c r="E144" t="n">
-        <v>59.85683624721152</v>
+        <v>59.85247805215541</v>
       </c>
     </row>
     <row r="145">
@@ -2891,16 +2891,16 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>11868.13972321</v>
+        <v>11868.14037220666</v>
       </c>
       <c r="C145" t="n">
-        <v>250.8602978814448</v>
+        <v>250.8602062994257</v>
       </c>
       <c r="D145" t="n">
-        <v>4.930955449943532e-05</v>
+        <v>0</v>
       </c>
       <c r="E145" t="n">
-        <v>52.53206484553159</v>
+        <v>52.53321829448757</v>
       </c>
     </row>
     <row r="146">
@@ -2908,16 +2908,16 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>11014.17001424026</v>
+        <v>11014.17025420971</v>
       </c>
       <c r="C146" t="n">
-        <v>182.8296935744613</v>
+        <v>182.8295712722838</v>
       </c>
       <c r="D146" t="n">
-        <v>0.0002918940377197216</v>
+        <v>0.0001743433734412435</v>
       </c>
       <c r="E146" t="n">
-        <v>30.54091419870934</v>
+        <v>30.54163368341024</v>
       </c>
     </row>
     <row r="147">
@@ -2925,16 +2925,16 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>9907.010095013797</v>
+        <v>9907.087301838374</v>
       </c>
       <c r="C147" t="n">
-        <v>195.9888671155039</v>
+        <v>195.983261354091</v>
       </c>
       <c r="D147" t="n">
-        <v>0.001036834796950291</v>
+        <v>0</v>
       </c>
       <c r="E147" t="n">
-        <v>26.31275545348162</v>
+        <v>26.30963213496167</v>
       </c>
     </row>
     <row r="148">
@@ -2942,16 +2942,16 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>10384.66682967247</v>
+        <v>10384.67629024488</v>
       </c>
       <c r="C148" t="n">
-        <v>226.3283430837937</v>
+        <v>226.3236123143575</v>
       </c>
       <c r="D148" t="n">
-        <v>0.004822423834664229</v>
+        <v>9.73427672853993e-05</v>
       </c>
       <c r="E148" t="n">
-        <v>28.33301406713605</v>
+        <v>28.32381939399506</v>
       </c>
     </row>
     <row r="149">
@@ -2959,16 +2959,16 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>10054.61936057063</v>
+        <v>10054.69735889103</v>
       </c>
       <c r="C149" t="n">
-        <v>271.3766144051494</v>
+        <v>271.3682540412491</v>
       </c>
       <c r="D149" t="n">
-        <v>0.004021006037456008</v>
+        <v>0</v>
       </c>
       <c r="E149" t="n">
-        <v>26.79721009363298</v>
+        <v>26.80717274111938</v>
       </c>
     </row>
     <row r="150">
@@ -2976,16 +2976,16 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>10107.06059881743</v>
+        <v>10106.95851865135</v>
       </c>
       <c r="C150" t="n">
-        <v>155.0269246029961</v>
+        <v>155.0370606985295</v>
       </c>
       <c r="D150" t="n">
-        <v>0</v>
+        <v>0.004416234346366127</v>
       </c>
       <c r="E150" t="n">
-        <v>26.96633856281488</v>
+        <v>26.95687294610562</v>
       </c>
     </row>
     <row r="151">
@@ -2993,16 +2993,16 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>10048.68180047317</v>
+        <v>10048.69171016909</v>
       </c>
       <c r="C151" t="n">
-        <v>332.3156990265583</v>
+        <v>332.3128268788881</v>
       </c>
       <c r="D151" t="n">
-        <v>0.002497998147372774</v>
+        <v>0</v>
       </c>
       <c r="E151" t="n">
-        <v>26.78645964852688</v>
+        <v>26.7901550250903</v>
       </c>
     </row>
     <row r="152">
@@ -3010,16 +3010,16 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>10277.85891816201</v>
+        <v>10277.80121113053</v>
       </c>
       <c r="C152" t="n">
-        <v>399.178162457464</v>
+        <v>399.1896270674339</v>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>0.009152646645571097</v>
       </c>
       <c r="E152" t="n">
-        <v>27.69988690534625</v>
+        <v>27.69637884813805</v>
       </c>
     </row>
     <row r="153">
@@ -3027,16 +3027,16 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>10754.29959001742</v>
+        <v>10754.47269055148</v>
       </c>
       <c r="C153" t="n">
-        <v>419.7985030655718</v>
+        <v>419.7852574166077</v>
       </c>
       <c r="D153" t="n">
         <v>0</v>
       </c>
       <c r="E153" t="n">
-        <v>29.09248664074841</v>
+        <v>29.09843795262325</v>
       </c>
     </row>
     <row r="154">
@@ -3044,16 +3044,16 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>11716.38528117251</v>
+        <v>11716.68166404444</v>
       </c>
       <c r="C154" t="n">
-        <v>342.5960744303286</v>
+        <v>342.5616002203375</v>
       </c>
       <c r="D154" t="n">
-        <v>0.01862578827076275</v>
+        <v>0</v>
       </c>
       <c r="E154" t="n">
-        <v>52.2844827310864</v>
+        <v>52.28379498530245</v>
       </c>
     </row>
     <row r="155">
@@ -3061,16 +3061,16 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>12728.33671336217</v>
+        <v>12728.35195178916</v>
       </c>
       <c r="C155" t="n">
-        <v>226.6635843985441</v>
+        <v>226.6625004747629</v>
       </c>
       <c r="D155" t="n">
         <v>0</v>
       </c>
       <c r="E155" t="n">
-        <v>58.39979667792367</v>
+        <v>58.3999839175102</v>
       </c>
     </row>
     <row r="156">
@@ -3078,16 +3078,16 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>13442.41782191931</v>
+        <v>13442.41794738479</v>
       </c>
       <c r="C156" t="n">
-        <v>151.5948204811198</v>
+        <v>151.5948059040701</v>
       </c>
       <c r="D156" t="n">
         <v>0</v>
       </c>
       <c r="E156" t="n">
-        <v>1782.54644463921</v>
+        <v>1781.743763651152</v>
       </c>
     </row>
     <row r="157">
@@ -3095,16 +3095,16 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>13895.21413355932</v>
+        <v>13895.21316238457</v>
       </c>
       <c r="C157" t="n">
-        <v>66.78667355723977</v>
+        <v>66.78679493005872</v>
       </c>
       <c r="D157" t="n">
-        <v>0</v>
+        <v>4.264335295945736e-05</v>
       </c>
       <c r="E157" t="n">
-        <v>59.69739697917009</v>
+        <v>59.69748163437747</v>
       </c>
     </row>
     <row r="158">
@@ -3112,7 +3112,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>14101.86933712526</v>
+        <v>14101.77988275943</v>
       </c>
       <c r="C158" t="n">
         <v>0</v>
@@ -3121,7 +3121,7 @@
         <v>0</v>
       </c>
       <c r="E158" t="n">
-        <v>670.7189016455652</v>
+        <v>730.7359461009554</v>
       </c>
     </row>
     <row r="159">
@@ -3129,16 +3129,16 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>14043.99999677241</v>
+        <v>14044.00021304511</v>
       </c>
       <c r="C159" t="n">
-        <v>1.092146753555528e-06</v>
+        <v>0</v>
       </c>
       <c r="D159" t="n">
-        <v>2.317409268756219e-06</v>
+        <v>0</v>
       </c>
       <c r="E159" t="n">
-        <v>59.84386568031914</v>
+        <v>59.84384129291725</v>
       </c>
     </row>
     <row r="160">
@@ -3146,16 +3146,16 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>13897.0000555626</v>
+        <v>13896.99996496891</v>
       </c>
       <c r="C160" t="n">
-        <v>0</v>
+        <v>1.149554612621918e-05</v>
       </c>
       <c r="D160" t="n">
-        <v>0</v>
+        <v>2.351198683376981e-05</v>
       </c>
       <c r="E160" t="n">
-        <v>59.70170036753832</v>
+        <v>59.70170499097728</v>
       </c>
     </row>
     <row r="161">
@@ -3163,7 +3163,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>13818.00007700683</v>
+        <v>13818.000221666</v>
       </c>
       <c r="C161" t="n">
         <v>0</v>
@@ -3172,7 +3172,7 @@
         <v>0</v>
       </c>
       <c r="E161" t="n">
-        <v>59.51335717135963</v>
+        <v>59.51335309539689</v>
       </c>
     </row>
     <row r="162">
@@ -3180,16 +3180,16 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>14043.99998723009</v>
+        <v>14043.9999763033</v>
       </c>
       <c r="C162" t="n">
-        <v>4.261040057385956e-06</v>
+        <v>7.853578105517956e-06</v>
       </c>
       <c r="D162" t="n">
-        <v>8.500306046139813e-06</v>
+        <v>1.582724645415843e-05</v>
       </c>
       <c r="E162" t="n">
-        <v>59.43200903252478</v>
+        <v>59.43201835328084</v>
       </c>
     </row>
     <row r="163">
@@ -3197,7 +3197,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>14535.00210647743</v>
+        <v>14535.00059506585</v>
       </c>
       <c r="C163" t="n">
         <v>0</v>
@@ -3206,7 +3206,7 @@
         <v>0</v>
       </c>
       <c r="E163" t="n">
-        <v>60.2241882191871</v>
+        <v>60.22409205070321</v>
       </c>
     </row>
     <row r="164">
@@ -3214,7 +3214,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>14997.2429727745</v>
+        <v>14997.05358944564</v>
       </c>
       <c r="C164" t="n">
         <v>0</v>
@@ -3223,7 +3223,7 @@
         <v>0</v>
       </c>
       <c r="E164" t="n">
-        <v>90.72868317818202</v>
+        <v>90.70432704271107</v>
       </c>
     </row>
     <row r="165">
@@ -3231,16 +3231,16 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>15633.96883102865</v>
+        <v>15633.99493543575</v>
       </c>
       <c r="C165" t="n">
-        <v>0.01038428226766613</v>
+        <v>0.001687056093314164</v>
       </c>
       <c r="D165" t="n">
-        <v>0.02076393094971309</v>
+        <v>0.003374134211673176</v>
       </c>
       <c r="E165" t="n">
-        <v>92.4249704801212</v>
+        <v>92.45025696129916</v>
       </c>
     </row>
     <row r="166">
@@ -3248,7 +3248,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>15558.80379404485</v>
+        <v>15558.80009090063</v>
       </c>
       <c r="C166" t="n">
         <v>0</v>
@@ -3257,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="E166" t="n">
-        <v>469.6117748824836</v>
+        <v>474.5713131460266</v>
       </c>
     </row>
     <row r="167">
@@ -3265,16 +3265,16 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>14650.00243164846</v>
+        <v>14649.99995126225</v>
       </c>
       <c r="C167" t="n">
-        <v>0</v>
+        <v>1.62708916197455e-05</v>
       </c>
       <c r="D167" t="n">
-        <v>0</v>
+        <v>3.243450148267645e-05</v>
       </c>
       <c r="E167" t="n">
-        <v>62.05268213130742</v>
+        <v>62.05271924454449</v>
       </c>
     </row>
     <row r="168">
@@ -3282,16 +3282,16 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>13469.99164255852</v>
+        <v>13470.02415121176</v>
       </c>
       <c r="C168" t="n">
-        <v>0.002784431583600891</v>
+        <v>0</v>
       </c>
       <c r="D168" t="n">
-        <v>0.005567444232851836</v>
+        <v>0</v>
       </c>
       <c r="E168" t="n">
-        <v>59.54291473389981</v>
+        <v>59.53766143929007</v>
       </c>
     </row>
     <row r="169">
@@ -3299,16 +3299,16 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>12277.99972719497</v>
+        <v>12278.00008663463</v>
       </c>
       <c r="C169" t="n">
-        <v>9.096088699695162e-05</v>
+        <v>8.216022754887822e-06</v>
       </c>
       <c r="D169" t="n">
-        <v>0.0001816626159306271</v>
+        <v>1.658659163167146e-05</v>
       </c>
       <c r="E169" t="n">
-        <v>90.25373166660823</v>
+        <v>90.25364444990682</v>
       </c>
     </row>
   </sheetData>

</xml_diff>